<commit_message>
update order thiết kế và source
</commit_message>
<xml_diff>
--- a/Bao_cao/Thiết kế/Thiết kế chi tiết/MILKTEAMANAGEMENT_TLPT_03_AddUser.xlsx
+++ b/Bao_cao/Thiết kế/Thiết kế chi tiết/MILKTEAMANAGEMENT_TLPT_03_AddUser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12210" tabRatio="826" activeTab="2"/>
+    <workbookView windowWidth="27945" windowHeight="12210" tabRatio="826" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_bìa" sheetId="19" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="Hinh1">"Thiết_kế!$R$7$1"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Thiết_kế!$A$1:$AW$106</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Trang_bìa!$A$1:$AW$156</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Xử lý chi tiết 10.9'!$A$1:$AW$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Xử lý chi tiết 10.9'!$A$1:$AW$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'機能間関連図 (2)'!$A:$AW</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -33249,10 +33249,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BF59"/>
+  <dimension ref="A1:BF57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="113" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46:AV46"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="113" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38:AV38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.66666666666667" defaultRowHeight="13.5" customHeight="1"/>
@@ -35282,956 +35282,956 @@
       <c r="C36" s="60"/>
       <c r="D36" s="61"/>
       <c r="E36" s="62"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="62"/>
-      <c r="J36" s="62"/>
-      <c r="K36" s="62"/>
-      <c r="L36" s="62"/>
-      <c r="M36" s="62"/>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
-      <c r="Q36" s="62"/>
-      <c r="R36" s="62"/>
-      <c r="S36" s="62"/>
-      <c r="T36" s="62"/>
-      <c r="U36" s="62"/>
-      <c r="V36" s="62"/>
-      <c r="W36" s="62"/>
-      <c r="X36" s="62"/>
-      <c r="Y36" s="62"/>
-      <c r="Z36" s="62"/>
-      <c r="AA36" s="62"/>
-      <c r="AB36" s="62"/>
-      <c r="AC36" s="62"/>
-      <c r="AD36" s="62"/>
-      <c r="AE36" s="62"/>
-      <c r="AF36" s="183"/>
-      <c r="AG36" s="62"/>
-      <c r="AH36" s="62"/>
-      <c r="AI36" s="62"/>
-      <c r="AJ36" s="62"/>
-      <c r="AK36" s="62"/>
-      <c r="AL36" s="62"/>
-      <c r="AM36" s="62"/>
-      <c r="AN36" s="62"/>
-      <c r="AO36" s="62"/>
-      <c r="AP36" s="62"/>
-      <c r="AQ36" s="62"/>
-      <c r="AR36" s="62"/>
-      <c r="AS36" s="62"/>
-      <c r="AT36" s="62"/>
-      <c r="AU36" s="62"/>
-      <c r="AV36" s="62"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="98"/>
+      <c r="K36" s="98"/>
+      <c r="L36" s="98"/>
+      <c r="M36" s="98"/>
+      <c r="N36" s="98"/>
+      <c r="O36" s="98"/>
+      <c r="P36" s="98"/>
+      <c r="Q36" s="98"/>
+      <c r="R36" s="98"/>
+      <c r="S36" s="98"/>
+      <c r="T36" s="98"/>
+      <c r="U36" s="98"/>
+      <c r="V36" s="98"/>
+      <c r="W36" s="98"/>
+      <c r="X36" s="98"/>
+      <c r="Y36" s="98"/>
+      <c r="Z36" s="98"/>
+      <c r="AA36" s="98"/>
+      <c r="AB36" s="98"/>
+      <c r="AC36" s="98"/>
+      <c r="AD36" s="98"/>
+      <c r="AE36" s="98"/>
+      <c r="AF36" s="184"/>
+      <c r="AG36" s="98"/>
+      <c r="AH36" s="98"/>
+      <c r="AI36" s="98"/>
+      <c r="AJ36" s="98"/>
+      <c r="AK36" s="98"/>
+      <c r="AL36" s="98"/>
+      <c r="AM36" s="98"/>
+      <c r="AN36" s="98"/>
+      <c r="AO36" s="98"/>
+      <c r="AP36" s="98"/>
+      <c r="AQ36" s="98"/>
+      <c r="AR36" s="98"/>
+      <c r="AS36" s="98"/>
+      <c r="AT36" s="98"/>
+      <c r="AU36" s="98"/>
+      <c r="AV36" s="98"/>
     </row>
     <row r="37" customHeight="1" spans="3:48">
       <c r="C37" s="60"/>
       <c r="D37" s="61"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
-      <c r="K37" s="62"/>
-      <c r="L37" s="62"/>
-      <c r="M37" s="62"/>
-      <c r="N37" s="62"/>
-      <c r="O37" s="62"/>
-      <c r="P37" s="62"/>
-      <c r="Q37" s="62"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="62"/>
-      <c r="T37" s="62"/>
-      <c r="U37" s="62"/>
-      <c r="V37" s="62"/>
-      <c r="W37" s="62"/>
-      <c r="X37" s="62"/>
-      <c r="Y37" s="62"/>
-      <c r="Z37" s="62"/>
-      <c r="AA37" s="62"/>
-      <c r="AB37" s="62"/>
-      <c r="AC37" s="62"/>
-      <c r="AD37" s="62"/>
-      <c r="AE37" s="62"/>
-      <c r="AF37" s="183"/>
-      <c r="AG37" s="62"/>
-      <c r="AH37" s="62"/>
-      <c r="AI37" s="62"/>
-      <c r="AJ37" s="62"/>
-      <c r="AK37" s="62"/>
-      <c r="AL37" s="62"/>
-      <c r="AM37" s="62"/>
-      <c r="AN37" s="62"/>
-      <c r="AO37" s="62"/>
-      <c r="AP37" s="62"/>
-      <c r="AQ37" s="62"/>
-      <c r="AR37" s="62"/>
-      <c r="AS37" s="62"/>
-      <c r="AT37" s="62"/>
-      <c r="AU37" s="62"/>
-      <c r="AV37" s="62"/>
+      <c r="E37" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" s="99"/>
+      <c r="G37" s="100"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
+      <c r="K37" s="100"/>
+      <c r="L37" s="100"/>
+      <c r="M37" s="100"/>
+      <c r="N37" s="100"/>
+      <c r="O37" s="100"/>
+      <c r="P37" s="100"/>
+      <c r="Q37" s="100"/>
+      <c r="R37" s="100"/>
+      <c r="S37" s="100"/>
+      <c r="T37" s="100"/>
+      <c r="U37" s="100"/>
+      <c r="V37" s="100"/>
+      <c r="W37" s="100"/>
+      <c r="X37" s="100"/>
+      <c r="Y37" s="100"/>
+      <c r="Z37" s="100"/>
+      <c r="AA37" s="100"/>
+      <c r="AB37" s="100"/>
+      <c r="AC37" s="100"/>
+      <c r="AD37" s="100"/>
+      <c r="AE37" s="100"/>
+      <c r="AF37" s="100"/>
+      <c r="AG37" s="100"/>
+      <c r="AH37" s="100"/>
+      <c r="AI37" s="100"/>
+      <c r="AJ37" s="100"/>
+      <c r="AK37" s="100"/>
+      <c r="AL37" s="100"/>
+      <c r="AM37" s="100"/>
+      <c r="AN37" s="100"/>
+      <c r="AO37" s="100"/>
+      <c r="AP37" s="100"/>
+      <c r="AQ37" s="100"/>
+      <c r="AR37" s="100"/>
+      <c r="AS37" s="100"/>
+      <c r="AT37" s="100"/>
+      <c r="AU37" s="100"/>
+      <c r="AV37" s="100"/>
     </row>
     <row r="38" customHeight="1" spans="3:48">
       <c r="C38" s="60"/>
       <c r="D38" s="61"/>
       <c r="E38" s="62"/>
-      <c r="F38" s="97"/>
-      <c r="G38" s="98"/>
-      <c r="H38" s="98"/>
-      <c r="I38" s="98"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="98"/>
-      <c r="L38" s="98"/>
-      <c r="M38" s="98"/>
-      <c r="N38" s="98"/>
-      <c r="O38" s="98"/>
-      <c r="P38" s="98"/>
-      <c r="Q38" s="98"/>
-      <c r="R38" s="98"/>
-      <c r="S38" s="98"/>
-      <c r="T38" s="98"/>
-      <c r="U38" s="98"/>
-      <c r="V38" s="98"/>
-      <c r="W38" s="98"/>
-      <c r="X38" s="98"/>
-      <c r="Y38" s="98"/>
-      <c r="Z38" s="98"/>
-      <c r="AA38" s="98"/>
-      <c r="AB38" s="98"/>
-      <c r="AC38" s="98"/>
-      <c r="AD38" s="98"/>
-      <c r="AE38" s="98"/>
-      <c r="AF38" s="184"/>
-      <c r="AG38" s="98"/>
-      <c r="AH38" s="98"/>
-      <c r="AI38" s="98"/>
-      <c r="AJ38" s="98"/>
-      <c r="AK38" s="98"/>
-      <c r="AL38" s="98"/>
-      <c r="AM38" s="98"/>
-      <c r="AN38" s="98"/>
-      <c r="AO38" s="98"/>
-      <c r="AP38" s="98"/>
-      <c r="AQ38" s="98"/>
-      <c r="AR38" s="98"/>
-      <c r="AS38" s="98"/>
-      <c r="AT38" s="98"/>
-      <c r="AU38" s="98"/>
-      <c r="AV38" s="98"/>
+      <c r="F38" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="102"/>
+      <c r="H38" s="102"/>
+      <c r="I38" s="102"/>
+      <c r="J38" s="102"/>
+      <c r="K38" s="102"/>
+      <c r="L38" s="140"/>
+      <c r="M38" s="141" t="s">
+        <v>142</v>
+      </c>
+      <c r="N38" s="142"/>
+      <c r="O38" s="142"/>
+      <c r="P38" s="142"/>
+      <c r="Q38" s="142"/>
+      <c r="R38" s="142"/>
+      <c r="S38" s="142"/>
+      <c r="T38" s="142"/>
+      <c r="U38" s="142"/>
+      <c r="V38" s="142"/>
+      <c r="W38" s="142"/>
+      <c r="X38" s="142"/>
+      <c r="Y38" s="142"/>
+      <c r="Z38" s="142"/>
+      <c r="AA38" s="142"/>
+      <c r="AB38" s="142"/>
+      <c r="AC38" s="142"/>
+      <c r="AD38" s="142"/>
+      <c r="AE38" s="142"/>
+      <c r="AF38" s="142"/>
+      <c r="AG38" s="142"/>
+      <c r="AH38" s="142"/>
+      <c r="AI38" s="142"/>
+      <c r="AJ38" s="142"/>
+      <c r="AK38" s="142"/>
+      <c r="AL38" s="142"/>
+      <c r="AM38" s="142"/>
+      <c r="AN38" s="142"/>
+      <c r="AO38" s="142"/>
+      <c r="AP38" s="142"/>
+      <c r="AQ38" s="142"/>
+      <c r="AR38" s="142"/>
+      <c r="AS38" s="142"/>
+      <c r="AT38" s="142"/>
+      <c r="AU38" s="142"/>
+      <c r="AV38" s="232"/>
     </row>
     <row r="39" customHeight="1" spans="3:48">
       <c r="C39" s="60"/>
       <c r="D39" s="61"/>
-      <c r="E39" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="F39" s="99"/>
-      <c r="G39" s="100"/>
-      <c r="H39" s="100"/>
-      <c r="I39" s="100"/>
-      <c r="J39" s="100"/>
-      <c r="K39" s="100"/>
-      <c r="L39" s="100"/>
-      <c r="M39" s="100"/>
-      <c r="N39" s="100"/>
-      <c r="O39" s="100"/>
-      <c r="P39" s="100"/>
-      <c r="Q39" s="100"/>
-      <c r="R39" s="100"/>
-      <c r="S39" s="100"/>
-      <c r="T39" s="100"/>
-      <c r="U39" s="100"/>
-      <c r="V39" s="100"/>
-      <c r="W39" s="100"/>
-      <c r="X39" s="100"/>
-      <c r="Y39" s="100"/>
-      <c r="Z39" s="100"/>
-      <c r="AA39" s="100"/>
-      <c r="AB39" s="100"/>
-      <c r="AC39" s="100"/>
-      <c r="AD39" s="100"/>
-      <c r="AE39" s="100"/>
-      <c r="AF39" s="100"/>
-      <c r="AG39" s="100"/>
-      <c r="AH39" s="100"/>
-      <c r="AI39" s="100"/>
-      <c r="AJ39" s="100"/>
-      <c r="AK39" s="100"/>
-      <c r="AL39" s="100"/>
-      <c r="AM39" s="100"/>
-      <c r="AN39" s="100"/>
-      <c r="AO39" s="100"/>
-      <c r="AP39" s="100"/>
-      <c r="AQ39" s="100"/>
-      <c r="AR39" s="100"/>
-      <c r="AS39" s="100"/>
-      <c r="AT39" s="100"/>
-      <c r="AU39" s="100"/>
-      <c r="AV39" s="100"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="G39" s="104"/>
+      <c r="H39" s="104"/>
+      <c r="I39" s="104"/>
+      <c r="J39" s="104"/>
+      <c r="K39" s="104"/>
+      <c r="L39" s="143"/>
+      <c r="M39" s="144"/>
+      <c r="N39" s="124"/>
+      <c r="O39" s="124" t="s">
+        <v>143</v>
+      </c>
+      <c r="P39" s="124"/>
+      <c r="Q39" s="124"/>
+      <c r="R39" s="164"/>
+      <c r="S39" s="164"/>
+      <c r="T39" s="164"/>
+      <c r="U39" s="164"/>
+      <c r="V39" s="164"/>
+      <c r="W39" s="164"/>
+      <c r="X39" s="164"/>
+      <c r="Y39" s="164"/>
+      <c r="Z39" s="164"/>
+      <c r="AA39" s="164"/>
+      <c r="AB39" s="164"/>
+      <c r="AC39" s="164"/>
+      <c r="AD39" s="164"/>
+      <c r="AE39" s="164"/>
+      <c r="AF39" s="164"/>
+      <c r="AG39" s="164"/>
+      <c r="AH39" s="164"/>
+      <c r="AI39" s="164"/>
+      <c r="AJ39" s="164"/>
+      <c r="AK39" s="164"/>
+      <c r="AL39" s="164"/>
+      <c r="AM39" s="164"/>
+      <c r="AN39" s="164"/>
+      <c r="AO39" s="164"/>
+      <c r="AP39" s="164"/>
+      <c r="AQ39" s="164"/>
+      <c r="AR39" s="164"/>
+      <c r="AS39" s="164"/>
+      <c r="AT39" s="164"/>
+      <c r="AU39" s="164"/>
+      <c r="AV39" s="197"/>
     </row>
     <row r="40" customHeight="1" spans="3:48">
       <c r="C40" s="60"/>
       <c r="D40" s="61"/>
       <c r="E40" s="62"/>
-      <c r="F40" s="101" t="s">
-        <v>141</v>
-      </c>
-      <c r="G40" s="102"/>
-      <c r="H40" s="102"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
-      <c r="K40" s="102"/>
-      <c r="L40" s="140"/>
-      <c r="M40" s="141" t="s">
-        <v>142</v>
-      </c>
-      <c r="N40" s="142"/>
-      <c r="O40" s="142"/>
-      <c r="P40" s="142"/>
-      <c r="Q40" s="142"/>
-      <c r="R40" s="142"/>
-      <c r="S40" s="142"/>
-      <c r="T40" s="142"/>
-      <c r="U40" s="142"/>
-      <c r="V40" s="142"/>
-      <c r="W40" s="142"/>
-      <c r="X40" s="142"/>
-      <c r="Y40" s="142"/>
-      <c r="Z40" s="142"/>
-      <c r="AA40" s="142"/>
-      <c r="AB40" s="142"/>
-      <c r="AC40" s="142"/>
-      <c r="AD40" s="142"/>
-      <c r="AE40" s="142"/>
-      <c r="AF40" s="142"/>
-      <c r="AG40" s="142"/>
-      <c r="AH40" s="142"/>
-      <c r="AI40" s="142"/>
-      <c r="AJ40" s="142"/>
-      <c r="AK40" s="142"/>
-      <c r="AL40" s="142"/>
-      <c r="AM40" s="142"/>
-      <c r="AN40" s="142"/>
-      <c r="AO40" s="142"/>
-      <c r="AP40" s="142"/>
-      <c r="AQ40" s="142"/>
-      <c r="AR40" s="142"/>
-      <c r="AS40" s="142"/>
-      <c r="AT40" s="142"/>
-      <c r="AU40" s="142"/>
-      <c r="AV40" s="232"/>
+      <c r="F40" s="105"/>
+      <c r="G40" s="106"/>
+      <c r="H40" s="106"/>
+      <c r="I40" s="106"/>
+      <c r="J40" s="106"/>
+      <c r="K40" s="106"/>
+      <c r="L40" s="145"/>
+      <c r="M40" s="146"/>
+      <c r="N40" s="147"/>
+      <c r="O40" s="147" t="s">
+        <v>144</v>
+      </c>
+      <c r="P40" s="147"/>
+      <c r="Q40" s="147"/>
+      <c r="R40" s="166"/>
+      <c r="S40" s="166"/>
+      <c r="T40" s="166"/>
+      <c r="U40" s="166"/>
+      <c r="V40" s="166"/>
+      <c r="W40" s="166"/>
+      <c r="X40" s="166"/>
+      <c r="Y40" s="166"/>
+      <c r="Z40" s="166"/>
+      <c r="AA40" s="166"/>
+      <c r="AB40" s="166"/>
+      <c r="AC40" s="166"/>
+      <c r="AD40" s="166"/>
+      <c r="AE40" s="166"/>
+      <c r="AF40" s="166"/>
+      <c r="AG40" s="166"/>
+      <c r="AH40" s="166"/>
+      <c r="AI40" s="166"/>
+      <c r="AJ40" s="166"/>
+      <c r="AK40" s="166"/>
+      <c r="AL40" s="166"/>
+      <c r="AM40" s="166"/>
+      <c r="AN40" s="166"/>
+      <c r="AO40" s="166"/>
+      <c r="AP40" s="166"/>
+      <c r="AQ40" s="166"/>
+      <c r="AR40" s="166"/>
+      <c r="AS40" s="166"/>
+      <c r="AT40" s="166"/>
+      <c r="AU40" s="166"/>
+      <c r="AV40" s="233"/>
     </row>
     <row r="41" customHeight="1" spans="3:48">
       <c r="C41" s="60"/>
       <c r="D41" s="61"/>
       <c r="E41" s="62"/>
-      <c r="F41" s="103" t="s">
-        <v>55</v>
-      </c>
-      <c r="G41" s="104"/>
-      <c r="H41" s="104"/>
-      <c r="I41" s="104"/>
-      <c r="J41" s="104"/>
-      <c r="K41" s="104"/>
-      <c r="L41" s="143"/>
-      <c r="M41" s="144"/>
-      <c r="N41" s="124"/>
-      <c r="O41" s="124" t="s">
-        <v>143</v>
-      </c>
-      <c r="P41" s="124"/>
-      <c r="Q41" s="124"/>
-      <c r="R41" s="164"/>
-      <c r="S41" s="164"/>
-      <c r="T41" s="164"/>
-      <c r="U41" s="164"/>
-      <c r="V41" s="164"/>
-      <c r="W41" s="164"/>
-      <c r="X41" s="164"/>
-      <c r="Y41" s="164"/>
-      <c r="Z41" s="164"/>
-      <c r="AA41" s="164"/>
-      <c r="AB41" s="164"/>
-      <c r="AC41" s="164"/>
-      <c r="AD41" s="164"/>
-      <c r="AE41" s="164"/>
-      <c r="AF41" s="164"/>
-      <c r="AG41" s="164"/>
-      <c r="AH41" s="164"/>
-      <c r="AI41" s="164"/>
-      <c r="AJ41" s="164"/>
-      <c r="AK41" s="164"/>
-      <c r="AL41" s="164"/>
-      <c r="AM41" s="164"/>
-      <c r="AN41" s="164"/>
-      <c r="AO41" s="164"/>
-      <c r="AP41" s="164"/>
-      <c r="AQ41" s="164"/>
-      <c r="AR41" s="164"/>
-      <c r="AS41" s="164"/>
-      <c r="AT41" s="164"/>
-      <c r="AU41" s="164"/>
-      <c r="AV41" s="197"/>
+      <c r="F41" s="107"/>
+      <c r="G41" s="108"/>
+      <c r="H41" s="108"/>
+      <c r="I41" s="108"/>
+      <c r="J41" s="108"/>
+      <c r="K41" s="108"/>
+      <c r="L41" s="148"/>
+      <c r="M41" s="149"/>
+      <c r="N41" s="136"/>
+      <c r="O41" s="136"/>
+      <c r="P41" s="136"/>
+      <c r="Q41" s="136"/>
+      <c r="R41" s="167"/>
+      <c r="S41" s="167"/>
+      <c r="T41" s="167"/>
+      <c r="U41" s="167"/>
+      <c r="V41" s="167"/>
+      <c r="W41" s="167"/>
+      <c r="X41" s="167"/>
+      <c r="Y41" s="167"/>
+      <c r="Z41" s="167"/>
+      <c r="AA41" s="167"/>
+      <c r="AB41" s="167"/>
+      <c r="AC41" s="167"/>
+      <c r="AD41" s="167"/>
+      <c r="AE41" s="167"/>
+      <c r="AF41" s="167"/>
+      <c r="AG41" s="167"/>
+      <c r="AH41" s="167"/>
+      <c r="AI41" s="167"/>
+      <c r="AJ41" s="167"/>
+      <c r="AK41" s="167"/>
+      <c r="AL41" s="167"/>
+      <c r="AM41" s="167"/>
+      <c r="AN41" s="167"/>
+      <c r="AO41" s="167"/>
+      <c r="AP41" s="167"/>
+      <c r="AQ41" s="167"/>
+      <c r="AR41" s="167"/>
+      <c r="AS41" s="167"/>
+      <c r="AT41" s="167"/>
+      <c r="AU41" s="167"/>
+      <c r="AV41" s="234"/>
     </row>
     <row r="42" customHeight="1" spans="3:48">
       <c r="C42" s="60"/>
       <c r="D42" s="61"/>
       <c r="E42" s="62"/>
-      <c r="F42" s="105"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="106"/>
-      <c r="J42" s="106"/>
-      <c r="K42" s="106"/>
-      <c r="L42" s="145"/>
-      <c r="M42" s="146"/>
-      <c r="N42" s="147"/>
-      <c r="O42" s="147" t="s">
-        <v>144</v>
-      </c>
-      <c r="P42" s="147"/>
-      <c r="Q42" s="147"/>
-      <c r="R42" s="166"/>
-      <c r="S42" s="166"/>
-      <c r="T42" s="166"/>
-      <c r="U42" s="166"/>
-      <c r="V42" s="166"/>
-      <c r="W42" s="166"/>
-      <c r="X42" s="166"/>
-      <c r="Y42" s="166"/>
-      <c r="Z42" s="166"/>
-      <c r="AA42" s="166"/>
-      <c r="AB42" s="166"/>
-      <c r="AC42" s="166"/>
-      <c r="AD42" s="166"/>
-      <c r="AE42" s="166"/>
-      <c r="AF42" s="166"/>
-      <c r="AG42" s="166"/>
-      <c r="AH42" s="166"/>
-      <c r="AI42" s="166"/>
-      <c r="AJ42" s="166"/>
-      <c r="AK42" s="166"/>
-      <c r="AL42" s="166"/>
-      <c r="AM42" s="166"/>
-      <c r="AN42" s="166"/>
-      <c r="AO42" s="166"/>
-      <c r="AP42" s="166"/>
-      <c r="AQ42" s="166"/>
-      <c r="AR42" s="166"/>
-      <c r="AS42" s="166"/>
-      <c r="AT42" s="166"/>
-      <c r="AU42" s="166"/>
-      <c r="AV42" s="233"/>
+      <c r="F42" s="97"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="62"/>
+      <c r="R42" s="62"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
+      <c r="U42" s="62"/>
+      <c r="V42" s="62"/>
+      <c r="W42" s="62"/>
+      <c r="X42" s="62"/>
+      <c r="Y42" s="62"/>
+      <c r="Z42" s="62"/>
+      <c r="AA42" s="98"/>
+      <c r="AB42" s="98"/>
+      <c r="AC42" s="98"/>
+      <c r="AD42" s="98"/>
+      <c r="AE42" s="98"/>
+      <c r="AF42" s="184"/>
+      <c r="AG42" s="98"/>
+      <c r="AH42" s="98"/>
+      <c r="AI42" s="98"/>
+      <c r="AJ42" s="98"/>
+      <c r="AK42" s="98"/>
+      <c r="AL42" s="98"/>
+      <c r="AM42" s="98"/>
+      <c r="AN42" s="98"/>
+      <c r="AO42" s="98"/>
+      <c r="AP42" s="98"/>
+      <c r="AQ42" s="98"/>
+      <c r="AR42" s="98"/>
+      <c r="AS42" s="98"/>
+      <c r="AT42" s="98"/>
+      <c r="AU42" s="98"/>
+      <c r="AV42" s="98"/>
     </row>
     <row r="43" customHeight="1" spans="3:48">
       <c r="C43" s="60"/>
       <c r="D43" s="61"/>
       <c r="E43" s="62"/>
-      <c r="F43" s="107"/>
-      <c r="G43" s="108"/>
-      <c r="H43" s="108"/>
-      <c r="I43" s="108"/>
-      <c r="J43" s="108"/>
-      <c r="K43" s="108"/>
-      <c r="L43" s="148"/>
-      <c r="M43" s="149"/>
-      <c r="N43" s="136"/>
-      <c r="O43" s="136"/>
-      <c r="P43" s="136"/>
-      <c r="Q43" s="136"/>
-      <c r="R43" s="167"/>
-      <c r="S43" s="167"/>
-      <c r="T43" s="167"/>
-      <c r="U43" s="167"/>
-      <c r="V43" s="167"/>
-      <c r="W43" s="167"/>
-      <c r="X43" s="167"/>
-      <c r="Y43" s="167"/>
-      <c r="Z43" s="167"/>
-      <c r="AA43" s="167"/>
-      <c r="AB43" s="167"/>
-      <c r="AC43" s="167"/>
-      <c r="AD43" s="167"/>
-      <c r="AE43" s="167"/>
-      <c r="AF43" s="167"/>
-      <c r="AG43" s="167"/>
-      <c r="AH43" s="167"/>
-      <c r="AI43" s="167"/>
-      <c r="AJ43" s="167"/>
-      <c r="AK43" s="167"/>
-      <c r="AL43" s="167"/>
-      <c r="AM43" s="167"/>
-      <c r="AN43" s="167"/>
-      <c r="AO43" s="167"/>
-      <c r="AP43" s="167"/>
-      <c r="AQ43" s="167"/>
-      <c r="AR43" s="167"/>
-      <c r="AS43" s="167"/>
-      <c r="AT43" s="167"/>
-      <c r="AU43" s="167"/>
-      <c r="AV43" s="234"/>
+      <c r="F43" s="99"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
+      <c r="U43" s="62"/>
+      <c r="V43" s="62"/>
+      <c r="W43" s="62"/>
+      <c r="X43" s="62"/>
+      <c r="Y43" s="62"/>
+      <c r="Z43" s="62"/>
+      <c r="AA43" s="98"/>
+      <c r="AB43" s="98"/>
+      <c r="AC43" s="98"/>
+      <c r="AD43" s="98"/>
+      <c r="AE43" s="98"/>
+      <c r="AF43" s="184"/>
+      <c r="AG43" s="98"/>
+      <c r="AH43" s="98"/>
+      <c r="AI43" s="98"/>
+      <c r="AJ43" s="98"/>
+      <c r="AK43" s="98"/>
+      <c r="AL43" s="98"/>
+      <c r="AM43" s="98"/>
+      <c r="AN43" s="98"/>
+      <c r="AO43" s="98"/>
+      <c r="AP43" s="98"/>
+      <c r="AQ43" s="98"/>
+      <c r="AR43" s="98"/>
+      <c r="AS43" s="98"/>
+      <c r="AT43" s="98"/>
+      <c r="AU43" s="98"/>
+      <c r="AV43" s="98"/>
     </row>
     <row r="44" customHeight="1" spans="3:48">
       <c r="C44" s="60"/>
       <c r="D44" s="61"/>
       <c r="E44" s="62"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62"/>
-      <c r="K44" s="62"/>
-      <c r="L44" s="62"/>
-      <c r="M44" s="62"/>
-      <c r="N44" s="62"/>
-      <c r="O44" s="62"/>
-      <c r="P44" s="62"/>
-      <c r="Q44" s="62"/>
-      <c r="R44" s="62"/>
-      <c r="S44" s="62"/>
-      <c r="T44" s="62"/>
-      <c r="U44" s="62"/>
-      <c r="V44" s="62"/>
-      <c r="W44" s="62"/>
-      <c r="X44" s="62"/>
-      <c r="Y44" s="62"/>
-      <c r="Z44" s="62"/>
-      <c r="AA44" s="98"/>
-      <c r="AB44" s="98"/>
-      <c r="AC44" s="98"/>
-      <c r="AD44" s="98"/>
-      <c r="AE44" s="98"/>
-      <c r="AF44" s="184"/>
-      <c r="AG44" s="98"/>
-      <c r="AH44" s="98"/>
-      <c r="AI44" s="98"/>
-      <c r="AJ44" s="98"/>
-      <c r="AK44" s="98"/>
-      <c r="AL44" s="98"/>
-      <c r="AM44" s="98"/>
-      <c r="AN44" s="98"/>
-      <c r="AO44" s="98"/>
-      <c r="AP44" s="98"/>
-      <c r="AQ44" s="98"/>
-      <c r="AR44" s="98"/>
-      <c r="AS44" s="98"/>
-      <c r="AT44" s="98"/>
-      <c r="AU44" s="98"/>
-      <c r="AV44" s="98"/>
+      <c r="F44" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="102"/>
+      <c r="H44" s="102"/>
+      <c r="I44" s="102"/>
+      <c r="J44" s="102"/>
+      <c r="K44" s="102"/>
+      <c r="L44" s="140"/>
+      <c r="M44" s="141" t="s">
+        <v>142</v>
+      </c>
+      <c r="N44" s="142"/>
+      <c r="O44" s="142"/>
+      <c r="P44" s="142"/>
+      <c r="Q44" s="142"/>
+      <c r="R44" s="142"/>
+      <c r="S44" s="142"/>
+      <c r="T44" s="142"/>
+      <c r="U44" s="142"/>
+      <c r="V44" s="142"/>
+      <c r="W44" s="142"/>
+      <c r="X44" s="142"/>
+      <c r="Y44" s="142"/>
+      <c r="Z44" s="142"/>
+      <c r="AA44" s="142"/>
+      <c r="AB44" s="142"/>
+      <c r="AC44" s="142"/>
+      <c r="AD44" s="142"/>
+      <c r="AE44" s="142"/>
+      <c r="AF44" s="142"/>
+      <c r="AG44" s="142"/>
+      <c r="AH44" s="142"/>
+      <c r="AI44" s="142"/>
+      <c r="AJ44" s="142"/>
+      <c r="AK44" s="142"/>
+      <c r="AL44" s="142"/>
+      <c r="AM44" s="142"/>
+      <c r="AN44" s="142"/>
+      <c r="AO44" s="142"/>
+      <c r="AP44" s="142"/>
+      <c r="AQ44" s="142"/>
+      <c r="AR44" s="142"/>
+      <c r="AS44" s="142"/>
+      <c r="AT44" s="142"/>
+      <c r="AU44" s="142"/>
+      <c r="AV44" s="232"/>
     </row>
     <row r="45" customHeight="1" spans="3:48">
       <c r="C45" s="60"/>
       <c r="D45" s="61"/>
       <c r="E45" s="62"/>
-      <c r="F45" s="99"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="62"/>
-      <c r="K45" s="62"/>
-      <c r="L45" s="62"/>
-      <c r="M45" s="62"/>
-      <c r="N45" s="62"/>
-      <c r="O45" s="62"/>
-      <c r="P45" s="62"/>
-      <c r="Q45" s="62"/>
-      <c r="R45" s="62"/>
-      <c r="S45" s="62"/>
-      <c r="T45" s="62"/>
-      <c r="U45" s="62"/>
-      <c r="V45" s="62"/>
-      <c r="W45" s="62"/>
-      <c r="X45" s="62"/>
-      <c r="Y45" s="62"/>
-      <c r="Z45" s="62"/>
-      <c r="AA45" s="98"/>
-      <c r="AB45" s="98"/>
-      <c r="AC45" s="98"/>
-      <c r="AD45" s="98"/>
-      <c r="AE45" s="98"/>
-      <c r="AF45" s="184"/>
-      <c r="AG45" s="98"/>
-      <c r="AH45" s="98"/>
-      <c r="AI45" s="98"/>
-      <c r="AJ45" s="98"/>
-      <c r="AK45" s="98"/>
-      <c r="AL45" s="98"/>
-      <c r="AM45" s="98"/>
-      <c r="AN45" s="98"/>
-      <c r="AO45" s="98"/>
-      <c r="AP45" s="98"/>
-      <c r="AQ45" s="98"/>
-      <c r="AR45" s="98"/>
-      <c r="AS45" s="98"/>
-      <c r="AT45" s="98"/>
-      <c r="AU45" s="98"/>
-      <c r="AV45" s="98"/>
+      <c r="F45" s="103" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" s="104"/>
+      <c r="H45" s="104"/>
+      <c r="I45" s="104"/>
+      <c r="J45" s="104"/>
+      <c r="K45" s="104"/>
+      <c r="L45" s="143"/>
+      <c r="M45" s="144"/>
+      <c r="N45" s="124"/>
+      <c r="O45" s="124" t="s">
+        <v>146</v>
+      </c>
+      <c r="P45" s="124"/>
+      <c r="Q45" s="124"/>
+      <c r="R45" s="164"/>
+      <c r="S45" s="164"/>
+      <c r="T45" s="164"/>
+      <c r="U45" s="164"/>
+      <c r="V45" s="164"/>
+      <c r="W45" s="164"/>
+      <c r="X45" s="164"/>
+      <c r="Y45" s="164"/>
+      <c r="Z45" s="164"/>
+      <c r="AA45" s="164"/>
+      <c r="AB45" s="164"/>
+      <c r="AC45" s="164"/>
+      <c r="AD45" s="164"/>
+      <c r="AE45" s="164"/>
+      <c r="AF45" s="164"/>
+      <c r="AG45" s="164"/>
+      <c r="AH45" s="164"/>
+      <c r="AI45" s="164"/>
+      <c r="AJ45" s="164"/>
+      <c r="AK45" s="164"/>
+      <c r="AL45" s="164"/>
+      <c r="AM45" s="164"/>
+      <c r="AN45" s="164"/>
+      <c r="AO45" s="164"/>
+      <c r="AP45" s="164"/>
+      <c r="AQ45" s="164"/>
+      <c r="AR45" s="164"/>
+      <c r="AS45" s="164"/>
+      <c r="AT45" s="164"/>
+      <c r="AU45" s="164"/>
+      <c r="AV45" s="197"/>
     </row>
     <row r="46" customHeight="1" spans="3:48">
       <c r="C46" s="60"/>
       <c r="D46" s="61"/>
       <c r="E46" s="62"/>
-      <c r="F46" s="101" t="s">
-        <v>141</v>
-      </c>
-      <c r="G46" s="102"/>
-      <c r="H46" s="102"/>
-      <c r="I46" s="102"/>
-      <c r="J46" s="102"/>
-      <c r="K46" s="102"/>
-      <c r="L46" s="140"/>
-      <c r="M46" s="141" t="s">
-        <v>142</v>
-      </c>
-      <c r="N46" s="142"/>
-      <c r="O46" s="142"/>
-      <c r="P46" s="142"/>
-      <c r="Q46" s="142"/>
-      <c r="R46" s="142"/>
-      <c r="S46" s="142"/>
-      <c r="T46" s="142"/>
-      <c r="U46" s="142"/>
-      <c r="V46" s="142"/>
-      <c r="W46" s="142"/>
-      <c r="X46" s="142"/>
-      <c r="Y46" s="142"/>
-      <c r="Z46" s="142"/>
-      <c r="AA46" s="142"/>
-      <c r="AB46" s="142"/>
-      <c r="AC46" s="142"/>
-      <c r="AD46" s="142"/>
-      <c r="AE46" s="142"/>
-      <c r="AF46" s="142"/>
-      <c r="AG46" s="142"/>
-      <c r="AH46" s="142"/>
-      <c r="AI46" s="142"/>
-      <c r="AJ46" s="142"/>
-      <c r="AK46" s="142"/>
-      <c r="AL46" s="142"/>
-      <c r="AM46" s="142"/>
-      <c r="AN46" s="142"/>
-      <c r="AO46" s="142"/>
-      <c r="AP46" s="142"/>
-      <c r="AQ46" s="142"/>
-      <c r="AR46" s="142"/>
-      <c r="AS46" s="142"/>
-      <c r="AT46" s="142"/>
-      <c r="AU46" s="142"/>
-      <c r="AV46" s="232"/>
+      <c r="F46" s="105"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="106"/>
+      <c r="I46" s="106"/>
+      <c r="J46" s="106"/>
+      <c r="K46" s="106"/>
+      <c r="L46" s="145"/>
+      <c r="M46" s="146"/>
+      <c r="N46" s="147"/>
+      <c r="O46" s="147" t="s">
+        <v>147</v>
+      </c>
+      <c r="P46" s="147"/>
+      <c r="Q46" s="147"/>
+      <c r="R46" s="166"/>
+      <c r="S46" s="166"/>
+      <c r="T46" s="166"/>
+      <c r="U46" s="166"/>
+      <c r="V46" s="166"/>
+      <c r="W46" s="166"/>
+      <c r="X46" s="166"/>
+      <c r="Y46" s="166"/>
+      <c r="Z46" s="166"/>
+      <c r="AA46" s="166"/>
+      <c r="AB46" s="166"/>
+      <c r="AC46" s="166"/>
+      <c r="AD46" s="166"/>
+      <c r="AE46" s="166"/>
+      <c r="AF46" s="166"/>
+      <c r="AG46" s="166"/>
+      <c r="AH46" s="166"/>
+      <c r="AI46" s="166"/>
+      <c r="AJ46" s="166"/>
+      <c r="AK46" s="166"/>
+      <c r="AL46" s="166"/>
+      <c r="AM46" s="166"/>
+      <c r="AN46" s="166"/>
+      <c r="AO46" s="166"/>
+      <c r="AP46" s="166"/>
+      <c r="AQ46" s="166"/>
+      <c r="AR46" s="166"/>
+      <c r="AS46" s="166"/>
+      <c r="AT46" s="166"/>
+      <c r="AU46" s="166"/>
+      <c r="AV46" s="233"/>
     </row>
     <row r="47" customHeight="1" spans="3:48">
       <c r="C47" s="60"/>
       <c r="D47" s="61"/>
       <c r="E47" s="62"/>
-      <c r="F47" s="103" t="s">
-        <v>145</v>
-      </c>
-      <c r="G47" s="104"/>
-      <c r="H47" s="104"/>
-      <c r="I47" s="104"/>
-      <c r="J47" s="104"/>
-      <c r="K47" s="104"/>
-      <c r="L47" s="143"/>
-      <c r="M47" s="144"/>
-      <c r="N47" s="124"/>
-      <c r="O47" s="124" t="s">
-        <v>146</v>
-      </c>
-      <c r="P47" s="124"/>
-      <c r="Q47" s="124"/>
-      <c r="R47" s="164"/>
-      <c r="S47" s="164"/>
-      <c r="T47" s="164"/>
-      <c r="U47" s="164"/>
-      <c r="V47" s="164"/>
-      <c r="W47" s="164"/>
-      <c r="X47" s="164"/>
-      <c r="Y47" s="164"/>
-      <c r="Z47" s="164"/>
-      <c r="AA47" s="164"/>
-      <c r="AB47" s="164"/>
-      <c r="AC47" s="164"/>
-      <c r="AD47" s="164"/>
-      <c r="AE47" s="164"/>
-      <c r="AF47" s="164"/>
-      <c r="AG47" s="164"/>
-      <c r="AH47" s="164"/>
-      <c r="AI47" s="164"/>
-      <c r="AJ47" s="164"/>
-      <c r="AK47" s="164"/>
-      <c r="AL47" s="164"/>
-      <c r="AM47" s="164"/>
-      <c r="AN47" s="164"/>
-      <c r="AO47" s="164"/>
-      <c r="AP47" s="164"/>
-      <c r="AQ47" s="164"/>
-      <c r="AR47" s="164"/>
-      <c r="AS47" s="164"/>
-      <c r="AT47" s="164"/>
-      <c r="AU47" s="164"/>
-      <c r="AV47" s="197"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="108"/>
+      <c r="H47" s="108"/>
+      <c r="I47" s="108"/>
+      <c r="J47" s="108"/>
+      <c r="K47" s="108"/>
+      <c r="L47" s="148"/>
+      <c r="M47" s="149"/>
+      <c r="N47" s="136"/>
+      <c r="O47" s="136"/>
+      <c r="P47" s="136"/>
+      <c r="Q47" s="136"/>
+      <c r="R47" s="167"/>
+      <c r="S47" s="167"/>
+      <c r="T47" s="167"/>
+      <c r="U47" s="167"/>
+      <c r="V47" s="167"/>
+      <c r="W47" s="167"/>
+      <c r="X47" s="167"/>
+      <c r="Y47" s="167"/>
+      <c r="Z47" s="167"/>
+      <c r="AA47" s="167"/>
+      <c r="AB47" s="167"/>
+      <c r="AC47" s="167"/>
+      <c r="AD47" s="167"/>
+      <c r="AE47" s="167"/>
+      <c r="AF47" s="167"/>
+      <c r="AG47" s="167"/>
+      <c r="AH47" s="167"/>
+      <c r="AI47" s="167"/>
+      <c r="AJ47" s="167"/>
+      <c r="AK47" s="167"/>
+      <c r="AL47" s="167"/>
+      <c r="AM47" s="167"/>
+      <c r="AN47" s="167"/>
+      <c r="AO47" s="167"/>
+      <c r="AP47" s="167"/>
+      <c r="AQ47" s="167"/>
+      <c r="AR47" s="167"/>
+      <c r="AS47" s="167"/>
+      <c r="AT47" s="167"/>
+      <c r="AU47" s="167"/>
+      <c r="AV47" s="234"/>
     </row>
     <row r="48" customHeight="1" spans="3:48">
       <c r="C48" s="60"/>
       <c r="D48" s="61"/>
-      <c r="E48" s="62"/>
-      <c r="F48" s="105"/>
-      <c r="G48" s="106"/>
-      <c r="H48" s="106"/>
-      <c r="I48" s="106"/>
-      <c r="J48" s="106"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="145"/>
-      <c r="M48" s="146"/>
-      <c r="N48" s="147"/>
-      <c r="O48" s="147" t="s">
-        <v>147</v>
-      </c>
-      <c r="P48" s="147"/>
-      <c r="Q48" s="147"/>
-      <c r="R48" s="166"/>
-      <c r="S48" s="166"/>
-      <c r="T48" s="166"/>
-      <c r="U48" s="166"/>
-      <c r="V48" s="166"/>
-      <c r="W48" s="166"/>
-      <c r="X48" s="166"/>
-      <c r="Y48" s="166"/>
-      <c r="Z48" s="166"/>
-      <c r="AA48" s="166"/>
-      <c r="AB48" s="166"/>
-      <c r="AC48" s="166"/>
-      <c r="AD48" s="166"/>
-      <c r="AE48" s="166"/>
-      <c r="AF48" s="166"/>
-      <c r="AG48" s="166"/>
-      <c r="AH48" s="166"/>
-      <c r="AI48" s="166"/>
-      <c r="AJ48" s="166"/>
-      <c r="AK48" s="166"/>
-      <c r="AL48" s="166"/>
-      <c r="AM48" s="166"/>
-      <c r="AN48" s="166"/>
-      <c r="AO48" s="166"/>
-      <c r="AP48" s="166"/>
-      <c r="AQ48" s="166"/>
-      <c r="AR48" s="166"/>
-      <c r="AS48" s="166"/>
-      <c r="AT48" s="166"/>
-      <c r="AU48" s="166"/>
-      <c r="AV48" s="233"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="577" t="s">
+        <v>148</v>
+      </c>
+      <c r="H48" s="98"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="98"/>
+      <c r="M48" s="98"/>
+      <c r="N48" s="98"/>
+      <c r="O48" s="98"/>
+      <c r="P48" s="98"/>
+      <c r="Q48" s="98"/>
+      <c r="R48" s="98"/>
+      <c r="S48" s="98"/>
+      <c r="T48" s="98"/>
+      <c r="U48" s="98"/>
+      <c r="V48" s="98"/>
+      <c r="W48" s="98"/>
+      <c r="X48" s="98"/>
+      <c r="Y48" s="98"/>
+      <c r="Z48" s="98"/>
+      <c r="AA48" s="98"/>
+      <c r="AB48" s="98"/>
+      <c r="AC48" s="98"/>
+      <c r="AD48" s="98"/>
+      <c r="AE48" s="98"/>
+      <c r="AF48" s="184"/>
+      <c r="AG48" s="98"/>
+      <c r="AH48" s="98"/>
+      <c r="AI48" s="98"/>
+      <c r="AJ48" s="98"/>
+      <c r="AK48" s="98"/>
+      <c r="AL48" s="98"/>
+      <c r="AM48" s="98"/>
+      <c r="AN48" s="98"/>
+      <c r="AO48" s="98"/>
+      <c r="AP48" s="98"/>
+      <c r="AQ48" s="98"/>
+      <c r="AR48" s="98"/>
+      <c r="AS48" s="98"/>
+      <c r="AT48" s="98"/>
+      <c r="AU48" s="98"/>
+      <c r="AV48" s="98"/>
     </row>
     <row r="49" customHeight="1" spans="3:48">
       <c r="C49" s="60"/>
       <c r="D49" s="61"/>
-      <c r="E49" s="62"/>
-      <c r="F49" s="107"/>
-      <c r="G49" s="108"/>
-      <c r="H49" s="108"/>
-      <c r="I49" s="108"/>
-      <c r="J49" s="108"/>
-      <c r="K49" s="108"/>
-      <c r="L49" s="148"/>
-      <c r="M49" s="149"/>
-      <c r="N49" s="136"/>
-      <c r="O49" s="136"/>
-      <c r="P49" s="136"/>
-      <c r="Q49" s="136"/>
-      <c r="R49" s="167"/>
-      <c r="S49" s="167"/>
-      <c r="T49" s="167"/>
-      <c r="U49" s="167"/>
-      <c r="V49" s="167"/>
-      <c r="W49" s="167"/>
-      <c r="X49" s="167"/>
-      <c r="Y49" s="167"/>
-      <c r="Z49" s="167"/>
-      <c r="AA49" s="167"/>
-      <c r="AB49" s="167"/>
-      <c r="AC49" s="167"/>
-      <c r="AD49" s="167"/>
-      <c r="AE49" s="167"/>
-      <c r="AF49" s="167"/>
-      <c r="AG49" s="167"/>
-      <c r="AH49" s="167"/>
-      <c r="AI49" s="167"/>
-      <c r="AJ49" s="167"/>
-      <c r="AK49" s="167"/>
-      <c r="AL49" s="167"/>
-      <c r="AM49" s="167"/>
-      <c r="AN49" s="167"/>
-      <c r="AO49" s="167"/>
-      <c r="AP49" s="167"/>
-      <c r="AQ49" s="167"/>
-      <c r="AR49" s="167"/>
-      <c r="AS49" s="167"/>
-      <c r="AT49" s="167"/>
-      <c r="AU49" s="167"/>
-      <c r="AV49" s="234"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="97"/>
+      <c r="G49" s="577" t="s">
+        <v>149</v>
+      </c>
+      <c r="H49" s="98"/>
+      <c r="I49" s="98"/>
+      <c r="J49" s="98"/>
+      <c r="K49" s="98"/>
+      <c r="L49" s="98"/>
+      <c r="M49" s="98"/>
+      <c r="N49" s="98"/>
+      <c r="O49" s="98"/>
+      <c r="P49" s="98"/>
+      <c r="Q49" s="98"/>
+      <c r="R49" s="98"/>
+      <c r="S49" s="98"/>
+      <c r="T49" s="98"/>
+      <c r="U49" s="98"/>
+      <c r="V49" s="98"/>
+      <c r="W49" s="98"/>
+      <c r="X49" s="98"/>
+      <c r="Y49" s="98"/>
+      <c r="Z49" s="98"/>
+      <c r="AA49" s="98"/>
+      <c r="AB49" s="98"/>
+      <c r="AC49" s="98"/>
+      <c r="AD49" s="98"/>
+      <c r="AE49" s="98"/>
+      <c r="AF49" s="184"/>
+      <c r="AG49" s="98"/>
+      <c r="AH49" s="98"/>
+      <c r="AI49" s="98"/>
+      <c r="AJ49" s="98"/>
+      <c r="AK49" s="98"/>
+      <c r="AL49" s="98"/>
+      <c r="AM49" s="98"/>
+      <c r="AN49" s="98"/>
+      <c r="AO49" s="98"/>
+      <c r="AP49" s="98"/>
+      <c r="AQ49" s="98"/>
+      <c r="AR49" s="98"/>
+      <c r="AS49" s="98"/>
+      <c r="AT49" s="98"/>
+      <c r="AU49" s="98"/>
+      <c r="AV49" s="98"/>
     </row>
     <row r="50" customHeight="1" spans="3:48">
       <c r="C50" s="60"/>
       <c r="D50" s="61"/>
       <c r="E50" s="83"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="577" t="s">
-        <v>148</v>
-      </c>
-      <c r="H50" s="98"/>
-      <c r="I50" s="98"/>
-      <c r="J50" s="98"/>
-      <c r="K50" s="98"/>
-      <c r="L50" s="98"/>
-      <c r="M50" s="98"/>
-      <c r="N50" s="98"/>
-      <c r="O50" s="98"/>
-      <c r="P50" s="98"/>
-      <c r="Q50" s="98"/>
-      <c r="R50" s="98"/>
-      <c r="S50" s="98"/>
-      <c r="T50" s="98"/>
-      <c r="U50" s="98"/>
-      <c r="V50" s="98"/>
-      <c r="W50" s="98"/>
-      <c r="X50" s="98"/>
-      <c r="Y50" s="98"/>
-      <c r="Z50" s="98"/>
-      <c r="AA50" s="98"/>
-      <c r="AB50" s="98"/>
-      <c r="AC50" s="98"/>
-      <c r="AD50" s="98"/>
-      <c r="AE50" s="98"/>
-      <c r="AF50" s="184"/>
-      <c r="AG50" s="98"/>
-      <c r="AH50" s="98"/>
-      <c r="AI50" s="98"/>
-      <c r="AJ50" s="98"/>
-      <c r="AK50" s="98"/>
-      <c r="AL50" s="98"/>
-      <c r="AM50" s="98"/>
-      <c r="AN50" s="98"/>
-      <c r="AO50" s="98"/>
-      <c r="AP50" s="98"/>
-      <c r="AQ50" s="98"/>
-      <c r="AR50" s="98"/>
-      <c r="AS50" s="98"/>
-      <c r="AT50" s="98"/>
-      <c r="AU50" s="98"/>
+      <c r="F50" s="109" t="s">
+        <v>150</v>
+      </c>
+      <c r="G50" s="110"/>
+      <c r="H50" s="110"/>
+      <c r="I50" s="150"/>
+      <c r="J50" s="101" t="s">
+        <v>151</v>
+      </c>
+      <c r="K50" s="102"/>
+      <c r="L50" s="102"/>
+      <c r="M50" s="102"/>
+      <c r="N50" s="102"/>
+      <c r="O50" s="102"/>
+      <c r="P50" s="102"/>
+      <c r="Q50" s="102"/>
+      <c r="R50" s="102"/>
+      <c r="S50" s="102"/>
+      <c r="T50" s="102"/>
+      <c r="U50" s="102"/>
+      <c r="V50" s="102"/>
+      <c r="W50" s="102"/>
+      <c r="X50" s="102"/>
+      <c r="Y50" s="102"/>
+      <c r="Z50" s="102"/>
+      <c r="AA50" s="102"/>
+      <c r="AB50" s="102"/>
+      <c r="AC50" s="102"/>
+      <c r="AD50" s="102"/>
+      <c r="AE50" s="102"/>
+      <c r="AF50" s="102"/>
+      <c r="AG50" s="102"/>
+      <c r="AH50" s="102"/>
+      <c r="AI50" s="102"/>
+      <c r="AJ50" s="140"/>
+      <c r="AK50" s="101" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL50" s="102"/>
+      <c r="AM50" s="102"/>
+      <c r="AN50" s="102"/>
+      <c r="AO50" s="102"/>
+      <c r="AP50" s="102"/>
+      <c r="AQ50" s="102"/>
+      <c r="AR50" s="102"/>
+      <c r="AS50" s="102"/>
+      <c r="AT50" s="102"/>
+      <c r="AU50" s="140"/>
       <c r="AV50" s="98"/>
     </row>
     <row r="51" customHeight="1" spans="3:48">
       <c r="C51" s="60"/>
       <c r="D51" s="61"/>
       <c r="E51" s="83"/>
-      <c r="F51" s="97"/>
-      <c r="G51" s="577" t="s">
-        <v>149</v>
-      </c>
-      <c r="H51" s="98"/>
-      <c r="I51" s="98"/>
-      <c r="J51" s="98"/>
-      <c r="K51" s="98"/>
-      <c r="L51" s="98"/>
-      <c r="M51" s="98"/>
-      <c r="N51" s="98"/>
-      <c r="O51" s="98"/>
-      <c r="P51" s="98"/>
-      <c r="Q51" s="98"/>
-      <c r="R51" s="98"/>
-      <c r="S51" s="98"/>
-      <c r="T51" s="98"/>
-      <c r="U51" s="98"/>
-      <c r="V51" s="98"/>
-      <c r="W51" s="98"/>
-      <c r="X51" s="98"/>
-      <c r="Y51" s="98"/>
-      <c r="Z51" s="98"/>
-      <c r="AA51" s="98"/>
-      <c r="AB51" s="98"/>
-      <c r="AC51" s="98"/>
-      <c r="AD51" s="98"/>
-      <c r="AE51" s="98"/>
-      <c r="AF51" s="184"/>
-      <c r="AG51" s="98"/>
-      <c r="AH51" s="98"/>
-      <c r="AI51" s="98"/>
-      <c r="AJ51" s="98"/>
-      <c r="AK51" s="98"/>
-      <c r="AL51" s="98"/>
-      <c r="AM51" s="98"/>
-      <c r="AN51" s="98"/>
-      <c r="AO51" s="98"/>
-      <c r="AP51" s="98"/>
-      <c r="AQ51" s="98"/>
-      <c r="AR51" s="98"/>
-      <c r="AS51" s="98"/>
-      <c r="AT51" s="98"/>
-      <c r="AU51" s="98"/>
+      <c r="F51" s="111" t="s">
+        <v>153</v>
+      </c>
+      <c r="G51" s="112"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="151"/>
+      <c r="J51" s="152" t="s">
+        <v>154</v>
+      </c>
+      <c r="K51" s="153"/>
+      <c r="L51" s="153"/>
+      <c r="M51" s="153"/>
+      <c r="N51" s="153"/>
+      <c r="O51" s="153"/>
+      <c r="P51" s="153"/>
+      <c r="Q51" s="153"/>
+      <c r="R51" s="153"/>
+      <c r="S51" s="153"/>
+      <c r="T51" s="153"/>
+      <c r="U51" s="153"/>
+      <c r="V51" s="153"/>
+      <c r="W51" s="153"/>
+      <c r="X51" s="153"/>
+      <c r="Y51" s="153"/>
+      <c r="Z51" s="153"/>
+      <c r="AA51" s="153"/>
+      <c r="AB51" s="153"/>
+      <c r="AC51" s="153"/>
+      <c r="AD51" s="153"/>
+      <c r="AE51" s="153"/>
+      <c r="AF51" s="185"/>
+      <c r="AG51" s="153"/>
+      <c r="AH51" s="153"/>
+      <c r="AI51" s="153"/>
+      <c r="AJ51" s="209"/>
+      <c r="AK51" s="198" t="s">
+        <v>155</v>
+      </c>
+      <c r="AL51" s="153"/>
+      <c r="AM51" s="153"/>
+      <c r="AN51" s="153"/>
+      <c r="AO51" s="153"/>
+      <c r="AP51" s="153"/>
+      <c r="AQ51" s="153"/>
+      <c r="AR51" s="153"/>
+      <c r="AS51" s="153"/>
+      <c r="AT51" s="153"/>
+      <c r="AU51" s="209"/>
       <c r="AV51" s="98"/>
     </row>
     <row r="52" customHeight="1" spans="3:48">
       <c r="C52" s="60"/>
       <c r="D52" s="61"/>
       <c r="E52" s="83"/>
-      <c r="F52" s="109" t="s">
-        <v>150</v>
-      </c>
-      <c r="G52" s="110"/>
-      <c r="H52" s="110"/>
-      <c r="I52" s="150"/>
-      <c r="J52" s="101" t="s">
-        <v>151</v>
-      </c>
-      <c r="K52" s="102"/>
-      <c r="L52" s="102"/>
-      <c r="M52" s="102"/>
-      <c r="N52" s="102"/>
-      <c r="O52" s="102"/>
-      <c r="P52" s="102"/>
-      <c r="Q52" s="102"/>
-      <c r="R52" s="102"/>
-      <c r="S52" s="102"/>
-      <c r="T52" s="102"/>
-      <c r="U52" s="102"/>
-      <c r="V52" s="102"/>
-      <c r="W52" s="102"/>
-      <c r="X52" s="102"/>
-      <c r="Y52" s="102"/>
-      <c r="Z52" s="102"/>
-      <c r="AA52" s="102"/>
-      <c r="AB52" s="102"/>
-      <c r="AC52" s="102"/>
-      <c r="AD52" s="102"/>
-      <c r="AE52" s="102"/>
-      <c r="AF52" s="102"/>
-      <c r="AG52" s="102"/>
-      <c r="AH52" s="102"/>
-      <c r="AI52" s="102"/>
-      <c r="AJ52" s="140"/>
-      <c r="AK52" s="101" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL52" s="102"/>
-      <c r="AM52" s="102"/>
-      <c r="AN52" s="102"/>
-      <c r="AO52" s="102"/>
-      <c r="AP52" s="102"/>
-      <c r="AQ52" s="102"/>
-      <c r="AR52" s="102"/>
-      <c r="AS52" s="102"/>
-      <c r="AT52" s="102"/>
-      <c r="AU52" s="140"/>
+      <c r="F52" s="113" t="s">
+        <v>156</v>
+      </c>
+      <c r="G52" s="114"/>
+      <c r="H52" s="114"/>
+      <c r="I52" s="154"/>
+      <c r="J52" s="155" t="s">
+        <v>157</v>
+      </c>
+      <c r="K52" s="156"/>
+      <c r="L52" s="156"/>
+      <c r="M52" s="156"/>
+      <c r="N52" s="156"/>
+      <c r="O52" s="156"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
+      <c r="U52" s="156"/>
+      <c r="V52" s="156"/>
+      <c r="W52" s="156"/>
+      <c r="X52" s="156"/>
+      <c r="Y52" s="156"/>
+      <c r="Z52" s="156"/>
+      <c r="AA52" s="156"/>
+      <c r="AB52" s="156"/>
+      <c r="AC52" s="156"/>
+      <c r="AD52" s="156"/>
+      <c r="AE52" s="156"/>
+      <c r="AF52" s="186"/>
+      <c r="AG52" s="156"/>
+      <c r="AH52" s="156"/>
+      <c r="AI52" s="156"/>
+      <c r="AJ52" s="210"/>
+      <c r="AK52" s="211" t="s">
+        <v>158</v>
+      </c>
+      <c r="AL52" s="156"/>
+      <c r="AM52" s="156"/>
+      <c r="AN52" s="156"/>
+      <c r="AO52" s="156"/>
+      <c r="AP52" s="156"/>
+      <c r="AQ52" s="156"/>
+      <c r="AR52" s="156"/>
+      <c r="AS52" s="156"/>
+      <c r="AT52" s="156"/>
+      <c r="AU52" s="210"/>
       <c r="AV52" s="98"/>
     </row>
     <row r="53" customHeight="1" spans="3:48">
       <c r="C53" s="60"/>
       <c r="D53" s="61"/>
       <c r="E53" s="83"/>
-      <c r="F53" s="111" t="s">
-        <v>153</v>
-      </c>
-      <c r="G53" s="112"/>
-      <c r="H53" s="112"/>
-      <c r="I53" s="151"/>
-      <c r="J53" s="152" t="s">
-        <v>154</v>
-      </c>
-      <c r="K53" s="153"/>
-      <c r="L53" s="153"/>
-      <c r="M53" s="153"/>
-      <c r="N53" s="153"/>
-      <c r="O53" s="153"/>
-      <c r="P53" s="153"/>
-      <c r="Q53" s="153"/>
-      <c r="R53" s="153"/>
-      <c r="S53" s="153"/>
-      <c r="T53" s="153"/>
-      <c r="U53" s="153"/>
-      <c r="V53" s="153"/>
-      <c r="W53" s="153"/>
-      <c r="X53" s="153"/>
-      <c r="Y53" s="153"/>
-      <c r="Z53" s="153"/>
-      <c r="AA53" s="153"/>
-      <c r="AB53" s="153"/>
-      <c r="AC53" s="153"/>
-      <c r="AD53" s="153"/>
-      <c r="AE53" s="153"/>
-      <c r="AF53" s="185"/>
-      <c r="AG53" s="153"/>
-      <c r="AH53" s="153"/>
-      <c r="AI53" s="153"/>
-      <c r="AJ53" s="209"/>
-      <c r="AK53" s="198" t="s">
-        <v>155</v>
-      </c>
-      <c r="AL53" s="153"/>
-      <c r="AM53" s="153"/>
-      <c r="AN53" s="153"/>
-      <c r="AO53" s="153"/>
-      <c r="AP53" s="153"/>
-      <c r="AQ53" s="153"/>
-      <c r="AR53" s="153"/>
-      <c r="AS53" s="153"/>
-      <c r="AT53" s="153"/>
-      <c r="AU53" s="209"/>
+      <c r="F53" s="98"/>
+      <c r="G53" s="98"/>
+      <c r="H53" s="98"/>
+      <c r="I53" s="98"/>
+      <c r="J53" s="98"/>
+      <c r="K53" s="98"/>
+      <c r="L53" s="98"/>
+      <c r="M53" s="98"/>
+      <c r="N53" s="98"/>
+      <c r="O53" s="98"/>
+      <c r="P53" s="98"/>
+      <c r="Q53" s="98"/>
+      <c r="R53" s="98"/>
+      <c r="S53" s="98"/>
+      <c r="T53" s="98"/>
+      <c r="U53" s="98"/>
+      <c r="V53" s="98"/>
+      <c r="W53" s="98"/>
+      <c r="X53" s="98"/>
+      <c r="Y53" s="98"/>
+      <c r="Z53" s="98"/>
+      <c r="AA53" s="98"/>
+      <c r="AB53" s="98"/>
+      <c r="AC53" s="98"/>
+      <c r="AD53" s="98"/>
+      <c r="AE53" s="98"/>
+      <c r="AF53" s="184"/>
+      <c r="AG53" s="98"/>
+      <c r="AH53" s="98"/>
+      <c r="AI53" s="98"/>
+      <c r="AJ53" s="98"/>
+      <c r="AK53" s="212"/>
+      <c r="AL53" s="98"/>
+      <c r="AM53" s="98"/>
+      <c r="AN53" s="98"/>
+      <c r="AO53" s="98"/>
+      <c r="AP53" s="98"/>
+      <c r="AQ53" s="98"/>
+      <c r="AR53" s="98"/>
+      <c r="AS53" s="98"/>
+      <c r="AT53" s="98"/>
+      <c r="AU53" s="98"/>
       <c r="AV53" s="98"/>
     </row>
     <row r="54" customHeight="1" spans="3:48">
       <c r="C54" s="60"/>
       <c r="D54" s="61"/>
       <c r="E54" s="83"/>
-      <c r="F54" s="113" t="s">
-        <v>156</v>
-      </c>
-      <c r="G54" s="114"/>
-      <c r="H54" s="114"/>
-      <c r="I54" s="154"/>
-      <c r="J54" s="155" t="s">
-        <v>157</v>
-      </c>
-      <c r="K54" s="156"/>
-      <c r="L54" s="156"/>
-      <c r="M54" s="156"/>
-      <c r="N54" s="156"/>
-      <c r="O54" s="156"/>
-      <c r="P54" s="156"/>
-      <c r="Q54" s="156"/>
-      <c r="R54" s="156"/>
-      <c r="S54" s="156"/>
-      <c r="T54" s="156"/>
-      <c r="U54" s="156"/>
-      <c r="V54" s="156"/>
-      <c r="W54" s="156"/>
-      <c r="X54" s="156"/>
-      <c r="Y54" s="156"/>
-      <c r="Z54" s="156"/>
-      <c r="AA54" s="156"/>
-      <c r="AB54" s="156"/>
-      <c r="AC54" s="156"/>
-      <c r="AD54" s="156"/>
-      <c r="AE54" s="156"/>
-      <c r="AF54" s="186"/>
-      <c r="AG54" s="156"/>
-      <c r="AH54" s="156"/>
-      <c r="AI54" s="156"/>
-      <c r="AJ54" s="210"/>
-      <c r="AK54" s="211" t="s">
-        <v>158</v>
-      </c>
-      <c r="AL54" s="156"/>
-      <c r="AM54" s="156"/>
-      <c r="AN54" s="156"/>
-      <c r="AO54" s="156"/>
-      <c r="AP54" s="156"/>
-      <c r="AQ54" s="156"/>
-      <c r="AR54" s="156"/>
-      <c r="AS54" s="156"/>
-      <c r="AT54" s="156"/>
-      <c r="AU54" s="210"/>
+      <c r="F54" s="98"/>
+      <c r="G54" s="98"/>
+      <c r="H54" s="98"/>
+      <c r="I54" s="98"/>
+      <c r="J54" s="98"/>
+      <c r="K54" s="98"/>
+      <c r="L54" s="98"/>
+      <c r="M54" s="98"/>
+      <c r="N54" s="98"/>
+      <c r="O54" s="98"/>
+      <c r="P54" s="98"/>
+      <c r="Q54" s="98"/>
+      <c r="R54" s="98"/>
+      <c r="S54" s="98"/>
+      <c r="T54" s="98"/>
+      <c r="U54" s="98"/>
+      <c r="V54" s="98"/>
+      <c r="W54" s="98"/>
+      <c r="X54" s="98"/>
+      <c r="Y54" s="98"/>
+      <c r="Z54" s="98"/>
+      <c r="AA54" s="98"/>
+      <c r="AB54" s="98"/>
+      <c r="AC54" s="98"/>
+      <c r="AD54" s="98"/>
+      <c r="AE54" s="98"/>
+      <c r="AF54" s="184"/>
+      <c r="AG54" s="98"/>
+      <c r="AH54" s="98"/>
+      <c r="AI54" s="98"/>
+      <c r="AJ54" s="98"/>
+      <c r="AK54" s="212"/>
+      <c r="AL54" s="98"/>
+      <c r="AM54" s="98"/>
+      <c r="AN54" s="98"/>
+      <c r="AO54" s="98"/>
+      <c r="AP54" s="98"/>
+      <c r="AQ54" s="98"/>
+      <c r="AR54" s="98"/>
+      <c r="AS54" s="98"/>
+      <c r="AT54" s="98"/>
+      <c r="AU54" s="98"/>
       <c r="AV54" s="98"/>
     </row>
     <row r="55" customHeight="1" spans="3:48">
@@ -36378,102 +36378,6 @@
       <c r="AU57" s="98"/>
       <c r="AV57" s="98"/>
     </row>
-    <row r="58" customHeight="1" spans="3:48">
-      <c r="C58" s="60"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="98"/>
-      <c r="G58" s="98"/>
-      <c r="H58" s="98"/>
-      <c r="I58" s="98"/>
-      <c r="J58" s="98"/>
-      <c r="K58" s="98"/>
-      <c r="L58" s="98"/>
-      <c r="M58" s="98"/>
-      <c r="N58" s="98"/>
-      <c r="O58" s="98"/>
-      <c r="P58" s="98"/>
-      <c r="Q58" s="98"/>
-      <c r="R58" s="98"/>
-      <c r="S58" s="98"/>
-      <c r="T58" s="98"/>
-      <c r="U58" s="98"/>
-      <c r="V58" s="98"/>
-      <c r="W58" s="98"/>
-      <c r="X58" s="98"/>
-      <c r="Y58" s="98"/>
-      <c r="Z58" s="98"/>
-      <c r="AA58" s="98"/>
-      <c r="AB58" s="98"/>
-      <c r="AC58" s="98"/>
-      <c r="AD58" s="98"/>
-      <c r="AE58" s="98"/>
-      <c r="AF58" s="184"/>
-      <c r="AG58" s="98"/>
-      <c r="AH58" s="98"/>
-      <c r="AI58" s="98"/>
-      <c r="AJ58" s="98"/>
-      <c r="AK58" s="212"/>
-      <c r="AL58" s="98"/>
-      <c r="AM58" s="98"/>
-      <c r="AN58" s="98"/>
-      <c r="AO58" s="98"/>
-      <c r="AP58" s="98"/>
-      <c r="AQ58" s="98"/>
-      <c r="AR58" s="98"/>
-      <c r="AS58" s="98"/>
-      <c r="AT58" s="98"/>
-      <c r="AU58" s="98"/>
-      <c r="AV58" s="98"/>
-    </row>
-    <row r="59" customHeight="1" spans="3:48">
-      <c r="C59" s="60"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="83"/>
-      <c r="F59" s="98"/>
-      <c r="G59" s="98"/>
-      <c r="H59" s="98"/>
-      <c r="I59" s="98"/>
-      <c r="J59" s="98"/>
-      <c r="K59" s="98"/>
-      <c r="L59" s="98"/>
-      <c r="M59" s="98"/>
-      <c r="N59" s="98"/>
-      <c r="O59" s="98"/>
-      <c r="P59" s="98"/>
-      <c r="Q59" s="98"/>
-      <c r="R59" s="98"/>
-      <c r="S59" s="98"/>
-      <c r="T59" s="98"/>
-      <c r="U59" s="98"/>
-      <c r="V59" s="98"/>
-      <c r="W59" s="98"/>
-      <c r="X59" s="98"/>
-      <c r="Y59" s="98"/>
-      <c r="Z59" s="98"/>
-      <c r="AA59" s="98"/>
-      <c r="AB59" s="98"/>
-      <c r="AC59" s="98"/>
-      <c r="AD59" s="98"/>
-      <c r="AE59" s="98"/>
-      <c r="AF59" s="184"/>
-      <c r="AG59" s="98"/>
-      <c r="AH59" s="98"/>
-      <c r="AI59" s="98"/>
-      <c r="AJ59" s="98"/>
-      <c r="AK59" s="212"/>
-      <c r="AL59" s="98"/>
-      <c r="AM59" s="98"/>
-      <c r="AN59" s="98"/>
-      <c r="AO59" s="98"/>
-      <c r="AP59" s="98"/>
-      <c r="AQ59" s="98"/>
-      <c r="AR59" s="98"/>
-      <c r="AS59" s="98"/>
-      <c r="AT59" s="98"/>
-      <c r="AU59" s="98"/>
-      <c r="AV59" s="98"/>
-    </row>
   </sheetData>
   <mergeCells count="28">
     <mergeCell ref="AM1:AN1"/>
@@ -36489,21 +36393,21 @@
     <mergeCell ref="AH3:AL3"/>
     <mergeCell ref="AM3:AW3"/>
     <mergeCell ref="O35:AJ35"/>
-    <mergeCell ref="F40:L40"/>
-    <mergeCell ref="M40:AV40"/>
-    <mergeCell ref="F46:L46"/>
-    <mergeCell ref="M46:AV46"/>
-    <mergeCell ref="J52:AJ52"/>
-    <mergeCell ref="AK52:AU52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F38:L38"/>
+    <mergeCell ref="M38:AV38"/>
+    <mergeCell ref="F44:L44"/>
+    <mergeCell ref="M44:AV44"/>
+    <mergeCell ref="J50:AJ50"/>
+    <mergeCell ref="AK50:AU50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
     <mergeCell ref="A1:I3"/>
     <mergeCell ref="J1:O3"/>
     <mergeCell ref="P1:U3"/>
     <mergeCell ref="V1:Z2"/>
     <mergeCell ref="AA1:AL2"/>
-    <mergeCell ref="F41:L43"/>
-    <mergeCell ref="F47:L49"/>
+    <mergeCell ref="F39:L41"/>
+    <mergeCell ref="F45:L47"/>
   </mergeCells>
   <pageMargins left="0.590551181102362" right="0.590551181102362" top="0.590551181102362" bottom="0.590551181102362" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="30" fitToHeight="0" orientation="landscape" verticalDpi="300"/>

</xml_diff>